<commit_message>
default label property - dash:LabelRole
</commit_message>
<xml_diff>
--- a/docs/how-to-configure/sparnatural-car-configuration.xlsx
+++ b/docs/how-to-configure/sparnatural-car-configuration.xlsx
@@ -784,6 +784,9 @@
     <t xml:space="preserve">Spécifie le symptôme associé à un code erreur.</t>
   </si>
   <si>
+    <t>datasources:list_rdfslabel_count</t>
+  </si>
+  <si>
     <t>odb:hasComponent</t>
   </si>
   <si>
@@ -1092,9 +1095,6 @@
   </si>
   <si>
     <t>core:LiteralListProperty</t>
-  </si>
-  <si>
-    <t>datasources:list_rdfslabel_count</t>
   </si>
   <si>
     <t>datasources:query_list_URI_count</t>
@@ -1485,7 +1485,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1566,7 +1566,9 @@
     <xf fontId="12" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="4" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="7" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1600,6 +1602,7 @@
     <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf fontId="4" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="13" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3291,7 +3294,7 @@
       <selection activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="12.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.00390625"/>
     <col customWidth="1" min="2" max="2" width="22.129999999999999"/>
@@ -6314,26 +6317,27 @@
   </sheetPr>
   <sheetViews>
     <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.379999999999999"/>
-    <col customWidth="1" min="2" max="2" width="18.25"/>
-    <col customWidth="1" min="3" max="3" width="27.28125"/>
+    <col customWidth="1" min="1" max="1" width="33.421875"/>
+    <col customWidth="1" min="2" max="2" width="30.140625"/>
+    <col customWidth="1" min="3" max="3" width="20.7109375"/>
     <col customWidth="1" hidden="1" min="4" max="4" width="13.28125"/>
-    <col customWidth="1" min="5" max="5" width="14.25"/>
+    <col customWidth="1" min="5" max="5" width="20.140625"/>
     <col customWidth="1" hidden="1" min="6" max="6" width="14.25"/>
-    <col customWidth="1" min="7" max="7" width="45.130000000000003"/>
+    <col customWidth="1" hidden="1" min="7" max="7" width="45.130000000000003"/>
     <col customWidth="1" hidden="1" min="8" max="8" width="40.880000000000003"/>
-    <col customWidth="1" hidden="1" min="9" max="12" width="14.25"/>
-    <col customWidth="1" min="13" max="13" width="22.421875"/>
+    <col customWidth="1" hidden="1" min="9" max="10" width="14.25"/>
+    <col customWidth="1" min="11" max="12" width="14.25"/>
+    <col customWidth="1" min="13" max="13" width="16.57421875"/>
     <col customWidth="1" hidden="1" min="14" max="14" width="14.25"/>
-    <col customWidth="1" min="15" max="15" width="35.5"/>
+    <col customWidth="1" min="15" max="15" width="27.7109375"/>
     <col customWidth="1" min="16" max="16" width="14.25"/>
-    <col customWidth="1" min="17" max="17" width="28.00390625"/>
+    <col customWidth="1" min="17" max="17" width="30.57421875"/>
     <col customWidth="1" min="18" max="18" width="20.8515625"/>
     <col customWidth="1" min="19" max="19" width="20.7109375"/>
     <col customWidth="1" min="20" max="20" width="20.57421875"/>
@@ -6344,7 +6348,7 @@
     <col customWidth="1" min="25" max="28" width="14.25"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15">
+    <row r="1" ht="25.5">
       <c r="A1" s="39" t="s">
         <v>18</v>
       </c>
@@ -6428,7 +6432,7 @@
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
     </row>
-    <row r="6" ht="165.75">
+    <row r="6" ht="191.25">
       <c r="A6" s="29" t="s">
         <v>109</v>
       </c>
@@ -6678,7 +6682,7 @@
       <c r="AB9" s="35"/>
       <c r="AC9" s="35"/>
     </row>
-    <row r="10" ht="15">
+    <row r="10" ht="14.25">
       <c r="A10" s="38" t="str">
         <f>CONCATENATE("this:",RIGHT(C10,LEN(C10)-SEARCH(":",C10)),"_",RIGHT(B10,LEN(B10)-SEARCH(":",B10)))</f>
         <v>this:Vehicle_hasManufacturer</v>
@@ -6738,7 +6742,7 @@
       <c r="AB10" s="35"/>
       <c r="AC10" s="35"/>
     </row>
-    <row r="11" ht="38.25">
+    <row r="11" ht="25.5">
       <c r="A11" s="38" t="s">
         <v>169</v>
       </c>
@@ -6793,7 +6797,7 @@
       <c r="AB11" s="35"/>
       <c r="AC11" s="35"/>
     </row>
-    <row r="12" ht="15">
+    <row r="12" ht="14.25">
       <c r="A12" s="38" t="str">
         <f>CONCATENATE("this:",RIGHT(C12,LEN(C12)-SEARCH(":",C12)),"_",RIGHT(B12,LEN(B12)-SEARCH(":",B12)))</f>
         <v>this:Vehicle_weightInKg</v>
@@ -6882,7 +6886,7 @@
       <c r="AB13" s="48"/>
       <c r="AC13" s="48"/>
     </row>
-    <row r="14" ht="15">
+    <row r="14" ht="14.25">
       <c r="A14" s="38" t="str">
         <f>CONCATENATE("this:",RIGHT(C14,LEN(C14)-SEARCH(":",C14)),"_",RIGHT(B14,LEN(B14)-SEARCH(":",B14)))</f>
         <v>this:Manufacturer_name</v>
@@ -6975,7 +6979,7 @@
       <c r="AB15" s="48"/>
       <c r="AC15" s="48"/>
     </row>
-    <row r="16" ht="15">
+    <row r="16" ht="14.25">
       <c r="A16" s="38" t="str">
         <f t="shared" ref="A16:A33" si="0">CONCATENATE("this:",RIGHT(C16,LEN(C16)-SEARCH(":",C16)),"_",RIGHT(B16,LEN(B16)-SEARCH(":",B16)))</f>
         <v>this:Diagnostic_diagnosticDate</v>
@@ -7094,7 +7098,7 @@
       <c r="AB17" s="35"/>
       <c r="AC17" s="35"/>
     </row>
-    <row r="18" ht="15">
+    <row r="18" ht="14.25">
       <c r="A18" s="38" t="str">
         <f t="shared" si="0"/>
         <v>this:Diagnostic_hasResults</v>
@@ -7147,7 +7151,7 @@
       <c r="AB18" s="35"/>
       <c r="AC18" s="35"/>
     </row>
-    <row r="19" ht="15">
+    <row r="19" ht="14.25">
       <c r="A19" s="38" t="str">
         <f t="shared" si="0"/>
         <v>this:Diagnostic_diagnosticPlace</v>
@@ -7444,7 +7448,7 @@
       <c r="AB24" s="48"/>
       <c r="AC24" s="48"/>
     </row>
-    <row r="25" ht="15">
+    <row r="25" ht="14.25">
       <c r="A25" s="38" t="str">
         <f t="shared" si="0"/>
         <v>this:ErrorCode_errorCode</v>
@@ -7538,7 +7542,9 @@
         <v>168</v>
       </c>
       <c r="P26" s="35"/>
-      <c r="Q26" s="3"/>
+      <c r="Q26" s="53" t="s">
+        <v>236</v>
+      </c>
       <c r="R26" s="3"/>
       <c r="S26" s="35"/>
       <c r="T26" s="3" t="b">
@@ -7560,7 +7566,7 @@
         <v>this:ErrorCode_hasComponent</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>81</v>
@@ -7569,16 +7575,16 @@
         <v>2</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I27" s="35"/>
       <c r="J27" s="35"/>
@@ -7595,7 +7601,7 @@
       </c>
       <c r="P27" s="35"/>
       <c r="Q27" s="53" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="R27" s="53"/>
       <c r="S27" s="35"/>
@@ -7614,10 +7620,10 @@
     </row>
     <row r="28" ht="25.5">
       <c r="A28" s="38" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>81</v>
@@ -7626,16 +7632,16 @@
         <v>3</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I28" s="35"/>
       <c r="J28" s="35"/>
@@ -7648,7 +7654,7 @@
       </c>
       <c r="N28" s="32"/>
       <c r="O28" s="32" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="P28" s="35"/>
       <c r="Q28" s="35"/>
@@ -7659,10 +7665,10 @@
       </c>
       <c r="U28" s="35"/>
       <c r="V28" s="54" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="W28" s="54" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X28" s="35"/>
       <c r="Y28" s="35"/>
@@ -7704,13 +7710,13 @@
       <c r="AB29" s="48"/>
       <c r="AC29" s="48"/>
     </row>
-    <row r="30" ht="15">
+    <row r="30" ht="14.25">
       <c r="A30" s="38" t="str">
         <f t="shared" si="0"/>
         <v>this:Symptom_label</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>88</v>
@@ -7719,16 +7725,16 @@
         <v>1</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H30" s="33" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I30" s="35">
         <v>1</v>
@@ -7740,12 +7746,12 @@
         <v>158</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M30" s="35"/>
       <c r="N30" s="35"/>
       <c r="O30" s="32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P30" s="35" t="s">
         <v>161</v>
@@ -7797,13 +7803,13 @@
       <c r="AB31" s="48"/>
       <c r="AC31" s="48"/>
     </row>
-    <row r="32" ht="15">
+    <row r="32" ht="14.25">
       <c r="A32" s="38" t="str">
         <f t="shared" si="0"/>
         <v>this:Component_componentCode</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C32" s="52" t="s">
         <v>95</v>
@@ -7812,16 +7818,16 @@
         <v>1</v>
       </c>
       <c r="E32" s="32" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H32" s="33" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I32" s="35">
         <v>1</v>
@@ -7838,7 +7844,7 @@
       <c r="M32" s="35"/>
       <c r="N32" s="35"/>
       <c r="O32" s="32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P32" s="35"/>
       <c r="Q32" s="35"/>
@@ -7857,13 +7863,13 @@
       <c r="AB32" s="35"/>
       <c r="AC32" s="35"/>
     </row>
-    <row r="33" ht="15">
+    <row r="33" ht="14.25">
       <c r="A33" s="38" t="str">
         <f t="shared" si="0"/>
         <v>this:Component_label</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C33" s="52" t="s">
         <v>95</v>
@@ -7872,16 +7878,16 @@
         <v>2</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H33" s="33" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I33" s="35">
         <v>1</v>
@@ -7891,12 +7897,12 @@
         <v>158</v>
       </c>
       <c r="L33" s="35" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M33" s="35"/>
       <c r="N33" s="35"/>
       <c r="O33" s="32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P33" s="35" t="s">
         <v>161</v>
@@ -7919,12 +7925,12 @@
       <c r="AB33" s="35"/>
       <c r="AC33" s="35"/>
     </row>
-    <row r="34" ht="38.25">
+    <row r="34" ht="25.5">
       <c r="A34" s="38" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C34" s="52" t="s">
         <v>95</v>
@@ -7933,16 +7939,16 @@
         <v>3</v>
       </c>
       <c r="E34" s="32" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H34" s="33" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I34" s="35"/>
       <c r="J34" s="35"/>
@@ -7955,7 +7961,7 @@
         <v>102</v>
       </c>
       <c r="O34" s="32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P34" s="35"/>
       <c r="Q34" s="35"/>
@@ -9650,15 +9656,15 @@
       <c r="A1" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="56" t="str">
         <f>Entities!B1</f>
         <v>https://data.mydomain.com/ontologies/sparnatural-config</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>108</v>
       </c>
       <c r="D1" s="28"/>
-      <c r="E1" s="56"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
@@ -9676,63 +9682,63 @@
       <c r="I2" s="28"/>
     </row>
     <row r="3" ht="91.5" customHeight="1">
-      <c r="A3" s="57" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="B3" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="C3" s="59" t="s">
         <v>270</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="D3" s="58" t="s">
         <v>271</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="E3" s="58" t="s">
         <v>272</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>273</v>
       </c>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="59" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="59" t="s">
+      <c r="C4" s="60" t="s">
         <v>274</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="D4" s="60" t="s">
         <v>275</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="E4" s="60" t="s">
         <v>276</v>
       </c>
-      <c r="G4" s="59" t="s">
-        <v>273</v>
-      </c>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="F4" s="60" t="s">
+        <v>277</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>274</v>
+      </c>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="B5" s="56" t="s">
-        <v>277</v>
+      <c r="B5" s="57" t="s">
+        <v>278</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>153</v>
@@ -9743,14 +9749,14 @@
       <c r="I5" s="28"/>
     </row>
     <row r="6" ht="276" customHeight="1">
-      <c r="A6" s="61" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6" s="62" t="s">
-        <v>277</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>279</v>
+      <c r="A6" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="35"/>
@@ -9760,14 +9766,14 @@
       <c r="I6" s="28"/>
     </row>
     <row r="7" ht="315" customHeight="1">
-      <c r="A7" s="64" t="s">
-        <v>246</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>277</v>
+      <c r="A7" s="65" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" s="63" t="s">
+        <v>278</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
@@ -9777,14 +9783,14 @@
       <c r="I7" s="28"/>
     </row>
     <row r="8" ht="333.75" customHeight="1">
-      <c r="A8" s="64" t="s">
-        <v>247</v>
-      </c>
-      <c r="B8" s="62" t="s">
-        <v>277</v>
+      <c r="A8" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" s="63" t="s">
+        <v>278</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
@@ -9795,7 +9801,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="28"/>
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
@@ -9806,7 +9812,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="28"/>
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
@@ -9817,7 +9823,7 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="28"/>
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -9828,7 +9834,7 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="28"/>
-      <c r="B12" s="56"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
@@ -9839,7 +9845,7 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="28"/>
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
@@ -9850,7 +9856,7 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="28"/>
-      <c r="B14" s="56"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -9861,7 +9867,7 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="28"/>
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
@@ -9872,7 +9878,7 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="28"/>
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
@@ -9883,7 +9889,7 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="28"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
@@ -9894,7 +9900,7 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="28"/>
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
@@ -9905,7 +9911,7 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="28"/>
-      <c r="B19" s="56"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
@@ -9916,7 +9922,7 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="28"/>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
@@ -9927,7 +9933,7 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="28"/>
-      <c r="B21" s="56"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
@@ -9938,7 +9944,7 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="28"/>
-      <c r="B22" s="56"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
@@ -9949,7 +9955,7 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="28"/>
-      <c r="B23" s="56"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
@@ -9960,7 +9966,7 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="28"/>
-      <c r="B24" s="56"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
@@ -10975,14 +10981,14 @@
       <c r="A1" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="40" t="str">
+      <c r="B1" s="56" t="str">
         <f>Entities!B1</f>
         <v>https://data.mydomain.com/ontologies/sparnatural-config</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="65"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="28"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -11000,144 +11006,144 @@
       <c r="E3" s="28"/>
     </row>
     <row r="4" ht="58.5" customHeight="1">
-      <c r="A4" s="57" t="s">
-        <v>282</v>
-      </c>
-      <c r="B4" s="57" t="s">
+      <c r="A4" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="C4" s="58" t="s">
-        <v>269</v>
-      </c>
-      <c r="D4" s="57" t="s">
+      <c r="B4" s="58" t="s">
         <v>284</v>
       </c>
+      <c r="C4" s="59" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>285</v>
+      </c>
       <c r="E4" s="28"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>273</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>285</v>
-      </c>
-      <c r="E5" s="60"/>
+      <c r="C5" s="60" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>286</v>
+      </c>
+      <c r="E5" s="61"/>
     </row>
     <row r="6" ht="160.5" customHeight="1">
       <c r="A6" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="B6" s="56" t="s">
         <v>287</v>
       </c>
+      <c r="B6" s="57" t="s">
+        <v>288</v>
+      </c>
       <c r="C6" s="45" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E6" s="28"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="28"/>
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="28"/>
       <c r="D7" s="45"/>
       <c r="E7" s="28"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="28"/>
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="28"/>
       <c r="D8" s="45"/>
       <c r="E8" s="28"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="28"/>
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="28"/>
       <c r="D9" s="45"/>
       <c r="E9" s="28"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="28"/>
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="28"/>
       <c r="D10" s="45"/>
       <c r="E10" s="28"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="28"/>
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="28"/>
       <c r="D11" s="45"/>
       <c r="E11" s="28"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="28"/>
-      <c r="B12" s="56"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="28"/>
       <c r="D12" s="45"/>
       <c r="E12" s="28"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="28"/>
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="28"/>
       <c r="D13" s="45"/>
       <c r="E13" s="28"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="28"/>
-      <c r="B14" s="56"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="28"/>
       <c r="D14" s="45"/>
       <c r="E14" s="28"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="28"/>
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="28"/>
       <c r="D15" s="45"/>
       <c r="E15" s="28"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="28"/>
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="28"/>
       <c r="D16" s="45"/>
       <c r="E16" s="28"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="28"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="28"/>
       <c r="D17" s="45"/>
       <c r="E17" s="28"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="28"/>
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="28"/>
       <c r="D18" s="45"/>
       <c r="E18" s="28"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="28"/>
-      <c r="B19" s="56"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="28"/>
       <c r="D19" s="45"/>
       <c r="E19" s="28"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="28"/>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="28"/>
       <c r="D20" s="45"/>
       <c r="E20" s="28"/>
@@ -13331,14 +13337,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="66" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>291</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>292</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="2">
@@ -13346,10 +13352,10 @@
         <v>160</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3">
@@ -13357,10 +13363,10 @@
         <v>168</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4">
@@ -13368,43 +13374,43 @@
         <v>192</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="36" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="36" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8">
@@ -13412,18 +13418,18 @@
         <v>175</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>310</v>
+        <v>236</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>311</v>
@@ -13453,7 +13459,7 @@
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>317</v>
@@ -13515,7 +13521,7 @@
         <v>329</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19">

</xml_diff>